<commit_message>
Few more changes to files
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://raidermailwright-my.sharepoint.com/personal/cox_366_wright_edu/Documents/GenericCampusTourCompany/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{DB18B25A-8E92-487B-8EAF-237E80A256F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1FBF96D-6E0A-49CC-9BBA-172C7CFEEBF2}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{DB18B25A-8E92-487B-8EAF-237E80A256F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7452DC5-EF05-4CEF-B13F-F439DFC31392}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{037B2FE2-6C72-4D73-B057-C3823F9830A0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="1" activeTab="1" xr2:uid="{037B2FE2-6C72-4D73-B057-C3823F9830A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="54">
   <si>
     <t>Generic Campus Tour Company</t>
   </si>
@@ -91,6 +91,9 @@
     <t>The user will be able to type or select and search two locations from a dropdown menu to display the fastest route between them on the 3D map.</t>
   </si>
   <si>
+    <t>Complete</t>
+  </si>
+  <si>
     <t>Nick and Jimmie</t>
   </si>
   <si>
@@ -139,6 +142,12 @@
     <t>Test with 2 valid entries / selections in the same building</t>
   </si>
   <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Krisitin</t>
+  </si>
+  <si>
     <t>Test with 2 valid entries / selections in the different buildings</t>
   </si>
   <si>
@@ -172,6 +181,9 @@
     <t>Test with 1 valid entry line</t>
   </si>
   <si>
+    <t>Complete*</t>
+  </si>
+  <si>
     <t>Test with 1 invalid entry line</t>
   </si>
   <si>
@@ -208,13 +220,7 @@
     <t>Test with 1 invalid room location node</t>
   </si>
   <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Krisitin</t>
+    <t>Pass*</t>
   </si>
 </sst>
 </file>
@@ -377,10 +383,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -810,22 +812,22 @@
         <v>9</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" s="4">
         <v>10</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="57" x14ac:dyDescent="0.45">
@@ -833,25 +835,25 @@
         <v>200</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="7">
         <v>8</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
@@ -859,25 +861,25 @@
         <v>300</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" s="10">
         <v>10</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -895,7 +897,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -928,19 +930,19 @@
     </row>
     <row r="2" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>1</v>
@@ -960,28 +962,28 @@
         <v>101</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="F3" s="4">
         <v>100</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="57" x14ac:dyDescent="0.45">
@@ -989,28 +991,28 @@
         <v>102</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="F4" s="4">
         <v>100</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
@@ -1018,28 +1020,28 @@
         <v>103</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="F5" s="4">
         <v>100</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
@@ -1047,28 +1049,28 @@
         <v>104</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="F6" s="4">
         <v>100</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
@@ -1076,28 +1078,28 @@
         <v>105</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="F7" s="4">
         <v>100</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
@@ -1105,28 +1107,28 @@
         <v>106</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="F8" s="4">
         <v>100</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
@@ -1134,28 +1136,28 @@
         <v>107</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="F9" s="4">
         <v>100</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
@@ -1163,28 +1165,28 @@
         <v>108</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="F10" s="4">
         <v>100</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="57" x14ac:dyDescent="0.45">
@@ -1192,28 +1194,28 @@
         <v>109</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="F11" s="4">
         <v>100</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="57" x14ac:dyDescent="0.45">
@@ -1221,28 +1223,28 @@
         <v>110</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="F12" s="4">
         <v>100</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
@@ -1250,28 +1252,28 @@
         <v>201</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F13" s="7">
         <v>200</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
@@ -1279,28 +1281,28 @@
         <v>202</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F14" s="7">
         <v>200</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
@@ -1308,28 +1310,28 @@
         <v>203</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F15" s="7">
         <v>200</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
@@ -1337,28 +1339,28 @@
         <v>204</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" s="7">
         <v>200</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
@@ -1366,28 +1368,28 @@
         <v>205</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F17" s="7">
         <v>200</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
@@ -1395,28 +1397,28 @@
         <v>206</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F18" s="7">
         <v>200</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
@@ -1424,28 +1426,28 @@
         <v>207</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F19" s="7">
         <v>200</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
@@ -1453,28 +1455,28 @@
         <v>208</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F20" s="7">
         <v>200</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
@@ -1482,28 +1484,28 @@
         <v>209</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F21" s="7">
         <v>200</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
@@ -1511,28 +1513,28 @@
         <v>301</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F22" s="10">
         <v>300</v>
       </c>
       <c r="G22" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
@@ -1540,28 +1542,28 @@
         <v>302</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F23" s="10">
         <v>300</v>
       </c>
       <c r="G23" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
@@ -1569,28 +1571,28 @@
         <v>303</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F24" s="10">
         <v>300</v>
       </c>
       <c r="G24" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
@@ -1598,28 +1600,28 @@
         <v>304</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F25" s="10">
         <v>300</v>
       </c>
       <c r="G25" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>